<commit_message>
prepare for the test
</commit_message>
<xml_diff>
--- a/reports/report.xlsx
+++ b/reports/report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Desktop/cp_variant/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Desktop/cp_variant/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365F0572-128B-C444-9FB1-CE76E1F99363}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108736E3-D3A3-4D41-98F0-A72A8668CC5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="14900" xr2:uid="{28A546BB-D934-D041-B323-5AE6C3602BBB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>lseek</t>
   </si>
@@ -57,6 +57,51 @@
   </si>
   <si>
     <t>munmep</t>
+  </si>
+  <si>
+    <t>open/write</t>
+  </si>
+  <si>
+    <t>mmap/memcpy</t>
+  </si>
+  <si>
+    <t>4096*1</t>
+  </si>
+  <si>
+    <t>4096*2</t>
+  </si>
+  <si>
+    <t>4096*4</t>
+  </si>
+  <si>
+    <t>4096*6</t>
+  </si>
+  <si>
+    <t>4096*8</t>
+  </si>
+  <si>
+    <t>4096*10</t>
+  </si>
+  <si>
+    <t>4096*20</t>
+  </si>
+  <si>
+    <t>4096*40</t>
+  </si>
+  <si>
+    <t>4096*80</t>
+  </si>
+  <si>
+    <t>4096*128</t>
+  </si>
+  <si>
+    <t>4096*256</t>
+  </si>
+  <si>
+    <t>4096*512</t>
+  </si>
+  <si>
+    <t>1.6GB</t>
   </si>
 </sst>
 </file>
@@ -90,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -198,6 +243,132 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -207,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -248,6 +419,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -563,18 +767,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B04664-3965-E145-B74E-45A7848E3730}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:G28"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
@@ -588,7 +797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="14">
         <v>64</v>
       </c>
@@ -602,7 +811,7 @@
         <v>152866</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
         <v>128</v>
       </c>
@@ -616,7 +825,7 @@
         <v>624496</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>256</v>
       </c>
@@ -629,9 +838,16 @@
       <c r="D4" s="15">
         <v>377616</v>
       </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="22"/>
+      <c r="N4" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="22"/>
+    </row>
+    <row r="5" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>512</v>
       </c>
@@ -644,8 +860,16 @@
       <c r="D5" s="15">
         <v>226341</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J5" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="26"/>
+      <c r="N5" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="26"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>1024</v>
       </c>
@@ -658,8 +882,22 @@
       <c r="D6" s="15">
         <v>166678</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I6" s="1"/>
+      <c r="J6" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
         <v>2048</v>
       </c>
@@ -672,8 +910,18 @@
       <c r="D7" s="15">
         <v>122987</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I7" s="1"/>
+      <c r="J7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="19"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="19"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="14">
         <v>4096</v>
       </c>
@@ -686,8 +934,16 @@
       <c r="D8" s="15">
         <v>108688</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J8" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="N8" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="19"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
         <v>8192</v>
       </c>
@@ -700,8 +956,16 @@
       <c r="D9" s="15">
         <v>73773</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="19"/>
+      <c r="N9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="19"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
         <v>16384</v>
       </c>
@@ -714,8 +978,16 @@
       <c r="D10" s="15">
         <v>49712</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="19"/>
+      <c r="N10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="19"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="14">
         <v>32768</v>
       </c>
@@ -728,8 +1000,16 @@
       <c r="D11" s="15">
         <v>34209</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="19"/>
+      <c r="N11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="19"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
         <v>65536</v>
       </c>
@@ -742,8 +1022,16 @@
       <c r="D12" s="15">
         <v>29755</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J12" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="19"/>
+      <c r="N12" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="19"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
         <v>131072</v>
       </c>
@@ -756,8 +1044,16 @@
       <c r="D13" s="15">
         <v>23879</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="19"/>
+      <c r="N13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="19"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="14">
         <v>262144</v>
       </c>
@@ -771,8 +1067,16 @@
         <v>23175</v>
       </c>
       <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="19"/>
+      <c r="N14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="19"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="14">
         <v>524288</v>
       </c>
@@ -785,8 +1089,16 @@
       <c r="D15" s="15">
         <v>23722</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J15" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="19"/>
+      <c r="N15" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="19"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="14">
         <v>1048576</v>
       </c>
@@ -799,8 +1111,16 @@
       <c r="D16" s="15">
         <v>18985</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J16" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="19"/>
+      <c r="N16" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="O16" s="19"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="14">
         <v>2097152</v>
       </c>
@@ -814,8 +1134,16 @@
         <v>20007</v>
       </c>
       <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J17" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="19"/>
+      <c r="N17" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17" s="19"/>
+    </row>
+    <row r="18" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>4194304</v>
       </c>
@@ -828,16 +1156,24 @@
       <c r="D18" s="15">
         <v>20788</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J18" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="21"/>
+      <c r="N18" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="21"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
         <v>5</v>
       </c>
@@ -857,7 +1193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B22" s="4">
         <v>60</v>
       </c>
@@ -877,7 +1213,7 @@
         <v>56940</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B23" s="4">
         <v>50</v>
       </c>
@@ -897,7 +1233,7 @@
         <v>37238</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B24" s="4">
         <v>49</v>
       </c>
@@ -917,7 +1253,7 @@
         <v>37515</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B25" s="4">
         <v>70</v>
       </c>
@@ -937,7 +1273,7 @@
         <v>34492</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B26" s="4">
         <v>47</v>
       </c>
@@ -957,7 +1293,7 @@
         <v>35421</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B27" s="4">
         <v>58</v>
       </c>
@@ -977,7 +1313,7 @@
         <v>34944</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
         <v>51</v>
       </c>
@@ -998,6 +1334,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="J4:K4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>